<commit_message>
resumed solving complex sql questions after joining Aakash as Data Analyst
</commit_message>
<xml_diff>
--- a/Ankitbansal Complex sql playlist/SQL complex playlist Ankit Bansal.xlsx
+++ b/Ankitbansal Complex sql playlist/SQL complex playlist Ankit Bansal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\SQL problems\Ankitbansal Complex sql playlist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\SQL problems\SQL_complex_questions\Ankitbansal Complex sql playlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BB3841-831D-4926-974E-6FF4AFD5FEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F9DD13-AB6C-4131-BE61-F3F880C5A235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{04D106E5-2FB2-4DB9-A7D9-75408D93F610}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{04D106E5-2FB2-4DB9-A7D9-75408D93F610}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Ankit Bansal complex SQL Question Playlist</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Video No.</t>
   </si>
   <si>
-    <t>Question title</t>
-  </si>
-  <si>
     <t>Solved on</t>
   </si>
   <si>
@@ -94,13 +91,22 @@
   </si>
   <si>
     <t>Q14_join_datediff</t>
+  </si>
+  <si>
+    <t>Q18_SCD_2</t>
+  </si>
+  <si>
+    <t>Lead window function, dateadd</t>
+  </si>
+  <si>
+    <t>Question title/ desciption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +114,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,17 +151,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -146,8 +184,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,342 +510,346 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF48A430-C925-41FF-85BF-9910EB1135C3}">
-  <dimension ref="C2:K21"/>
+  <dimension ref="C2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="3"/>
+    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="3:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="3:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
-        <v>1</v>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="5">
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="E4" s="6">
+        <v>45714</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="H4" s="5">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="4">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
+      <c r="C5" s="5">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="6">
         <v>45714</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="4">
-        <v>6</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="4">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="5">
         <v>10</v>
       </c>
+      <c r="D6" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="6">
-        <v>45714</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+        <v>45720</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="4">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="5">
         <v>11</v>
       </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="6">
-        <v>45720</v>
-      </c>
-      <c r="F7" s="4" t="s">
+        <v>45721</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
+        <v>8</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="5">
         <v>12</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="4">
-        <v>8</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="4">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="6">
         <v>45721</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4">
-        <v>8</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="F8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5">
+        <v>7</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="4">
-        <v>12</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>17</v>
+      <c r="C9" s="5">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E9" s="6">
-        <v>45721</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4">
+        <v>45722</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5">
         <v>7</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="I9" s="5">
+        <v>40</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="4">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
+      <c r="C10" s="5">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E10" s="6">
         <v>45722</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="5">
         <v>6</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="I10" s="5">
+        <v>40</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="5">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6">
+        <v>45795</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="5">
         <v>7</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I11" s="5">
         <v>40</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="4">
-        <v>14</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="6">
-        <v>45722</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="4">
-        <v>6</v>
-      </c>
-      <c r="I11" s="4">
-        <v>40</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>